<commit_message>
[ADD] last code was addded
</commit_message>
<xml_diff>
--- a/results/efficient_from_zero/classification_report.xlsx
+++ b/results/efficient_from_zero/classification_report.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -497,16 +497,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.1363636363636364</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.1978021978021978</v>
       </c>
     </row>
     <row r="4">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0625</v>
+        <v>0.06451612903225806</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2352941176470588</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="F4" t="n">
-        <v>0.09876543209876543</v>
+        <v>0.1008403361344538</v>
       </c>
     </row>
     <row r="5">
@@ -541,16 +541,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2</v>
+        <v>0.1063829787234043</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1298701298701299</v>
       </c>
     </row>
     <row r="6">
@@ -563,16 +563,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.05357142857142857</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.1016949152542373</v>
       </c>
     </row>
     <row r="7">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>

</xml_diff>